<commit_message>
not yet done wit PW report
</commit_message>
<xml_diff>
--- a/PW/Heat exchanger curve(pump on).xlsx
+++ b/PW/Heat exchanger curve(pump on).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WKieee\Desktop\Term3 2D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUTD Term 3\2D\green-fingers-2d\PW\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17253" windowHeight="5667"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Time/s</t>
   </si>
@@ -41,6 +41,12 @@
       </rPr>
       <t>°C</t>
     </r>
+  </si>
+  <si>
+    <t>deltaT</t>
+  </si>
+  <si>
+    <t>T_amb</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1230,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1255,18 +1261,17 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="5"/>
-            <c:dispRSqr val="1"/>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.3897419072615923E-2"/>
-                  <c:y val="0.19629301545640129"/>
+                  <c:x val="-0.30915171437392136"/>
+                  <c:y val="-2.4610454708030791E-2"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.000000000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1676,378 +1681,378 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$124</c:f>
+              <c:f>Sheet1!$D$2:$D$124</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="123"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>15.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.9</c:v>
+                  <c:v>15.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.8</c:v>
+                  <c:v>15.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.7</c:v>
+                  <c:v>15.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.6</c:v>
+                  <c:v>15.400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.5</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41.4</c:v>
+                  <c:v>15.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.3</c:v>
+                  <c:v>15.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41.2</c:v>
+                  <c:v>15.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41.1</c:v>
+                  <c:v>14.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41</c:v>
+                  <c:v>14.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40.9</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>14.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40.700000000000003</c:v>
+                  <c:v>14.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40.6</c:v>
+                  <c:v>14.400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40.5</c:v>
+                  <c:v>14.3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40.4</c:v>
+                  <c:v>14.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>14.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40.200000000000003</c:v>
+                  <c:v>14.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>40.1</c:v>
+                  <c:v>13.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>40</c:v>
+                  <c:v>13.8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>39.9</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>39.799999999999997</c:v>
+                  <c:v>13.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>39.700000000000003</c:v>
+                  <c:v>13.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>39.6</c:v>
+                  <c:v>13.400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>39.5</c:v>
+                  <c:v>13.3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>39.4</c:v>
+                  <c:v>13.2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>39.299999999999997</c:v>
+                  <c:v>13.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>39.200000000000003</c:v>
+                  <c:v>13.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>39.1</c:v>
+                  <c:v>12.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>39</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>38.9</c:v>
+                  <c:v>12.7</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>38.799999999999997</c:v>
+                  <c:v>12.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>38.700000000000003</c:v>
+                  <c:v>12.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>38.6</c:v>
+                  <c:v>12.400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>38.5</c:v>
+                  <c:v>12.3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>38.4</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>38.299999999999997</c:v>
+                  <c:v>12.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.200000000000003</c:v>
+                  <c:v>12.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>38.1</c:v>
+                  <c:v>11.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>38</c:v>
+                  <c:v>11.8</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>37.9</c:v>
+                  <c:v>11.7</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>37.799999999999898</c:v>
+                  <c:v>11.599999999999898</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>37.699999999999903</c:v>
+                  <c:v>11.499999999999904</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>37.599999999999902</c:v>
+                  <c:v>11.399999999999903</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>37.499999999999901</c:v>
+                  <c:v>11.299999999999901</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>37.399999999999899</c:v>
+                  <c:v>11.1999999999999</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>37.299999999999898</c:v>
+                  <c:v>11.099999999999898</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>37.199999999999903</c:v>
+                  <c:v>10.999999999999904</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>37.099999999999902</c:v>
+                  <c:v>10.899999999999903</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>36.999999999999901</c:v>
+                  <c:v>10.799999999999901</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>36.899999999999899</c:v>
+                  <c:v>10.6999999999999</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>36.799999999999898</c:v>
+                  <c:v>10.599999999999898</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>36.699999999999903</c:v>
+                  <c:v>10.499999999999904</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>36.599999999999902</c:v>
+                  <c:v>10.399999999999903</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>36.499999999999901</c:v>
+                  <c:v>10.299999999999901</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>36.399999999999899</c:v>
+                  <c:v>10.1999999999999</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>36.299999999999898</c:v>
+                  <c:v>10.099999999999898</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>36.199999999999903</c:v>
+                  <c:v>9.9999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>36.099999999999902</c:v>
+                  <c:v>9.8999999999999027</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>35.999999999999901</c:v>
+                  <c:v>9.7999999999999012</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>35.899999999999899</c:v>
+                  <c:v>9.6999999999998998</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>35.799999999999898</c:v>
+                  <c:v>9.5999999999998984</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>35.699999999999903</c:v>
+                  <c:v>9.4999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>35.599999999999902</c:v>
+                  <c:v>9.3999999999999027</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>35.499999999999901</c:v>
+                  <c:v>9.2999999999999012</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>35.399999999999899</c:v>
+                  <c:v>9.1999999999998998</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>35.299999999999898</c:v>
+                  <c:v>9.0999999999998984</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>35.199999999999903</c:v>
+                  <c:v>8.9999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>35.099999999999902</c:v>
+                  <c:v>8.8999999999999027</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>34.999999999999901</c:v>
+                  <c:v>8.7999999999999012</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>34.899999999999899</c:v>
+                  <c:v>8.6999999999998998</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>34.799999999999898</c:v>
+                  <c:v>8.5999999999998984</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>34.699999999999903</c:v>
+                  <c:v>8.4999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>34.599999999999902</c:v>
+                  <c:v>8.3999999999999027</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>34.499999999999901</c:v>
+                  <c:v>8.2999999999999012</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>34.399999999999899</c:v>
+                  <c:v>8.1999999999998998</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>34.299999999999898</c:v>
+                  <c:v>8.0999999999998984</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>34.199999999999903</c:v>
+                  <c:v>7.9999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>34.099999999999902</c:v>
+                  <c:v>7.8999999999999027</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>33.999999999999901</c:v>
+                  <c:v>7.7999999999999012</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>33.899999999999899</c:v>
+                  <c:v>7.6999999999998998</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>33.799999999999898</c:v>
+                  <c:v>7.5999999999998984</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>33.699999999999903</c:v>
+                  <c:v>7.4999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>33.599999999999902</c:v>
+                  <c:v>7.3999999999999027</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>33.499999999999901</c:v>
+                  <c:v>7.2999999999999012</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>33.399999999999899</c:v>
+                  <c:v>7.1999999999998998</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>33.299999999999898</c:v>
+                  <c:v>7.0999999999998984</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>33.199999999999903</c:v>
+                  <c:v>6.9999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>33.099999999999902</c:v>
+                  <c:v>6.8999999999999027</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>32.999999999999901</c:v>
+                  <c:v>6.7999999999999012</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>32.899999999999899</c:v>
+                  <c:v>6.6999999999998998</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>32.799999999999898</c:v>
+                  <c:v>6.5999999999998984</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>32.699999999999903</c:v>
+                  <c:v>6.4999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>32.599999999999902</c:v>
+                  <c:v>6.3999999999999027</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>32.499999999999901</c:v>
+                  <c:v>6.2999999999999012</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>32.399999999999899</c:v>
+                  <c:v>6.1999999999998998</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>32.299999999999898</c:v>
+                  <c:v>6.0999999999998984</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>32.199999999999903</c:v>
+                  <c:v>5.9999999999999041</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>32.099999999999902</c:v>
+                  <c:v>5.8999999999999027</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>31.999999999999901</c:v>
+                  <c:v>5.7999999999999012</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>31.899999999999899</c:v>
+                  <c:v>5.6999999999998998</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>31.799999999999901</c:v>
+                  <c:v>5.5999999999999019</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>31.6999999999999</c:v>
+                  <c:v>5.4999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>31.599999999999898</c:v>
+                  <c:v>5.3999999999998991</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>31.499999999999901</c:v>
+                  <c:v>5.2999999999999012</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>31.399999999999899</c:v>
+                  <c:v>5.1999999999998998</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>31.299999999999901</c:v>
+                  <c:v>5.0999999999999019</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>31.1999999999999</c:v>
+                  <c:v>4.9999999999999005</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>31.099999999999799</c:v>
+                  <c:v>4.8999999999997996</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>30.999999999999801</c:v>
+                  <c:v>4.7999999999998018</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>30.8999999999998</c:v>
+                  <c:v>4.6999999999998003</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>30.799999999999802</c:v>
+                  <c:v>4.5999999999998025</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>30.6999999999998</c:v>
+                  <c:v>4.499999999999801</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>30.599999999999799</c:v>
+                  <c:v>4.3999999999997996</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>30.499999999999801</c:v>
+                  <c:v>4.2999999999998018</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>30.3999999999998</c:v>
+                  <c:v>4.1999999999998003</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>30.299999999999802</c:v>
+                  <c:v>4.0999999999998025</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>30.1999999999998</c:v>
+                  <c:v>3.999999999999801</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>30.099999999999799</c:v>
+                  <c:v>3.8999999999997996</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>29.999999999999801</c:v>
+                  <c:v>3.7999999999998018</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>29.8999999999998</c:v>
+                  <c:v>3.6999999999998003</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>29.799999999999802</c:v>
+                  <c:v>3.5999999999998025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3502,15 +3507,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:colOff>421640</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>171027</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:colOff>604520</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>57573</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3835,1004 +3840,1508 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C124"/>
+  <dimension ref="B1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="3" max="3" width="13.5859375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B2">
         <v>53.43</v>
       </c>
       <c r="C2">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <f>C2-$E$2</f>
+        <v>15.8</v>
+      </c>
+      <c r="E2">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B3">
         <v>56.22</v>
       </c>
       <c r="C3">
         <v>41.9</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3-$E$2</f>
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B4">
         <v>57.17</v>
       </c>
       <c r="C4">
         <v>41.8</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>15.599999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B5">
         <v>59.01</v>
       </c>
       <c r="C5">
         <v>41.7</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>15.500000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B6">
         <v>61.01</v>
       </c>
       <c r="C6">
         <v>41.6</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>15.400000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B7">
         <v>63.71</v>
       </c>
       <c r="C7">
         <v>41.5</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B8">
         <v>64.67</v>
       </c>
       <c r="C8">
         <v>41.4</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B9">
         <v>67.48</v>
       </c>
       <c r="C9">
         <v>41.3</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>15.099999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B10">
         <v>69.22</v>
       </c>
       <c r="C10">
         <v>41.2</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>15.000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B11">
         <v>71.28</v>
       </c>
       <c r="C11">
         <v>41.1</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>14.900000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B12">
         <v>73.14</v>
       </c>
       <c r="C12">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B13">
         <v>75.930000000000007</v>
       </c>
       <c r="C13">
         <v>40.9</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B14">
         <v>78.73</v>
       </c>
       <c r="C14">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>14.599999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B15">
         <v>80.58</v>
       </c>
       <c r="C15">
         <v>40.700000000000003</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>14.500000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B16">
         <v>82.46</v>
       </c>
       <c r="C16">
         <v>40.6</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>14.400000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B17">
         <v>84.3</v>
       </c>
       <c r="C17">
         <v>40.5</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B18">
         <v>87.29</v>
       </c>
       <c r="C18">
         <v>40.4</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B19">
         <v>90.88</v>
       </c>
       <c r="C19">
         <v>40.299999999999997</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>14.099999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B20">
         <v>92.78</v>
       </c>
       <c r="C20">
         <v>40.200000000000003</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>14.000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B21">
         <v>95.57</v>
       </c>
       <c r="C21">
         <v>40.1</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>13.900000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B22">
         <v>98.43</v>
       </c>
       <c r="C22">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B23">
         <v>101.23</v>
       </c>
       <c r="C23">
         <v>39.9</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B24">
         <v>103.17</v>
       </c>
       <c r="C24">
         <v>39.799999999999997</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>13.599999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B25">
         <v>105.85</v>
       </c>
       <c r="C25">
         <v>39.700000000000003</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>13.500000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B26">
         <v>109.69</v>
       </c>
       <c r="C26">
         <v>39.6</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>13.400000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B27">
         <v>112.48</v>
       </c>
       <c r="C27">
         <v>39.5</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B28">
         <v>115.29</v>
       </c>
       <c r="C28">
         <v>39.4</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B29">
         <v>118.07</v>
       </c>
       <c r="C29">
         <v>39.299999999999997</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>13.099999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B30">
         <v>120.86</v>
       </c>
       <c r="C30">
         <v>39.200000000000003</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>13.000000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B31">
         <v>123.77</v>
       </c>
       <c r="C31">
         <v>39.1</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>12.900000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B32">
         <v>126.51</v>
       </c>
       <c r="C32">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B33">
         <v>131.25</v>
       </c>
       <c r="C33">
         <v>38.9</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B34">
         <v>132.06</v>
       </c>
       <c r="C34">
         <v>38.799999999999997</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>12.599999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B35">
         <v>136.82</v>
       </c>
       <c r="C35">
         <v>38.700000000000003</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>12.500000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B36">
         <v>139.62</v>
       </c>
       <c r="C36">
         <v>38.6</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>12.400000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B37">
         <v>143.38</v>
       </c>
       <c r="C37">
         <v>38.5</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B38">
         <v>147.12</v>
       </c>
       <c r="C38">
         <v>38.4</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B39">
         <v>150.03</v>
       </c>
       <c r="C39">
         <v>38.299999999999997</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>12.099999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B40">
         <v>154.63999999999999</v>
       </c>
       <c r="C40">
         <v>38.200000000000003</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>12.000000000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B41">
         <v>158.38</v>
       </c>
       <c r="C41">
         <v>38.1</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>11.900000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B42">
         <v>161.27000000000001</v>
       </c>
       <c r="C42">
         <v>38</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B43">
         <v>164.04</v>
       </c>
       <c r="C43">
         <v>37.9</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B44">
         <v>168.78</v>
       </c>
       <c r="C44">
         <v>37.799999999999898</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>11.599999999999898</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B45">
         <v>172.51</v>
       </c>
       <c r="C45">
         <v>37.699999999999903</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>11.499999999999904</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B46">
         <v>176.26</v>
       </c>
       <c r="C46">
         <v>37.599999999999902</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>11.399999999999903</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B47">
         <v>180.89</v>
       </c>
       <c r="C47">
         <v>37.499999999999901</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>11.299999999999901</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B48">
         <v>184.66</v>
       </c>
       <c r="C48">
         <v>37.399999999999899</v>
       </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>11.1999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B49">
         <v>188.4</v>
       </c>
       <c r="C49">
         <v>37.299999999999898</v>
       </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>11.099999999999898</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B50">
         <v>192.16</v>
       </c>
       <c r="C50">
         <v>37.199999999999903</v>
       </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>10.999999999999904</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B51">
         <v>195.93</v>
       </c>
       <c r="C51">
         <v>37.099999999999902</v>
       </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>10.899999999999903</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B52">
         <v>199.65</v>
       </c>
       <c r="C52">
         <v>36.999999999999901</v>
       </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>10.799999999999901</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B53">
         <v>204.36</v>
       </c>
       <c r="C53">
         <v>36.899999999999899</v>
       </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>10.6999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B54">
         <v>209.07</v>
       </c>
       <c r="C54">
         <v>36.799999999999898</v>
       </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>10.599999999999898</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B55">
         <v>212.74</v>
       </c>
       <c r="C55">
         <v>36.699999999999903</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>10.499999999999904</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B56">
         <v>218.4</v>
       </c>
       <c r="C56">
         <v>36.599999999999902</v>
       </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>10.399999999999903</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B57">
         <v>222.18</v>
       </c>
       <c r="C57">
         <v>36.499999999999901</v>
       </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>10.299999999999901</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B58">
         <v>226.87</v>
       </c>
       <c r="C58">
         <v>36.399999999999899</v>
       </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>10.1999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B59">
         <v>230.68</v>
       </c>
       <c r="C59">
         <v>36.299999999999898</v>
       </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>10.099999999999898</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B60">
         <v>236.2</v>
       </c>
       <c r="C60">
         <v>36.199999999999903</v>
       </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999041</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B61">
         <v>241.87</v>
       </c>
       <c r="C61">
         <v>36.099999999999902</v>
       </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>9.8999999999999027</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B62">
         <v>243.68</v>
       </c>
       <c r="C62">
         <v>35.999999999999901</v>
       </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>9.7999999999999012</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B63">
         <v>250.26</v>
       </c>
       <c r="C63">
         <v>35.899999999999899</v>
       </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>9.6999999999998998</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B64">
         <v>254.18</v>
       </c>
       <c r="C64">
         <v>35.799999999999898</v>
       </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>9.5999999999998984</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B65">
         <v>261.51</v>
       </c>
       <c r="C65">
         <v>35.699999999999903</v>
       </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>9.4999999999999041</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B66">
         <v>265.25</v>
       </c>
       <c r="C66">
         <v>35.599999999999902</v>
       </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>9.3999999999999027</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B67">
         <v>270.85000000000002</v>
       </c>
       <c r="C67">
         <v>35.499999999999901</v>
       </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <f t="shared" ref="D67:D124" si="1">C67-$E$2</f>
+        <v>9.2999999999999012</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B68">
         <v>273.72000000000003</v>
       </c>
       <c r="C68">
         <v>35.399999999999899</v>
       </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <f t="shared" si="1"/>
+        <v>9.1999999999998998</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B69">
         <v>280.24</v>
       </c>
       <c r="C69">
         <v>35.299999999999898</v>
       </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <f t="shared" si="1"/>
+        <v>9.0999999999998984</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B70">
         <v>286.82</v>
       </c>
       <c r="C70">
         <v>35.199999999999903</v>
       </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <f t="shared" si="1"/>
+        <v>8.9999999999999041</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B71">
         <v>290.64999999999998</v>
       </c>
       <c r="C71">
         <v>35.099999999999902</v>
       </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <f t="shared" si="1"/>
+        <v>8.8999999999999027</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B72">
         <v>297.2</v>
       </c>
       <c r="C72">
         <v>34.999999999999901</v>
       </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999012</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B73">
         <v>300.95</v>
       </c>
       <c r="C73">
         <v>34.899999999999899</v>
       </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <f t="shared" si="1"/>
+        <v>8.6999999999998998</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B74">
         <v>307.48</v>
       </c>
       <c r="C74">
         <v>34.799999999999898</v>
       </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <f t="shared" si="1"/>
+        <v>8.5999999999998984</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B75">
         <v>311.27999999999997</v>
       </c>
       <c r="C75">
         <v>34.699999999999903</v>
       </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <f t="shared" si="1"/>
+        <v>8.4999999999999041</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B76">
         <v>318.75</v>
       </c>
       <c r="C76">
         <v>34.599999999999902</v>
       </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <f t="shared" si="1"/>
+        <v>8.3999999999999027</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B77">
         <v>326.18</v>
       </c>
       <c r="C77">
         <v>34.499999999999901</v>
       </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <f t="shared" si="1"/>
+        <v>8.2999999999999012</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B78">
         <v>330.02</v>
       </c>
       <c r="C78">
         <v>34.399999999999899</v>
       </c>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <f t="shared" si="1"/>
+        <v>8.1999999999998998</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B79">
         <v>336.56</v>
       </c>
       <c r="C79">
         <v>34.299999999999898</v>
       </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <f t="shared" si="1"/>
+        <v>8.0999999999998984</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B80">
         <v>342.15</v>
       </c>
       <c r="C80">
         <v>34.199999999999903</v>
       </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <f t="shared" si="1"/>
+        <v>7.9999999999999041</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B81">
         <v>349.65</v>
       </c>
       <c r="C81">
         <v>34.099999999999902</v>
       </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>7.8999999999999027</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B82">
         <v>353.49</v>
       </c>
       <c r="C82">
         <v>33.999999999999901</v>
       </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>7.7999999999999012</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B83">
         <v>361.83</v>
       </c>
       <c r="C83">
         <v>33.899999999999899</v>
       </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>7.6999999999998998</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B84">
         <v>370.3</v>
       </c>
       <c r="C84">
         <v>33.799999999999898</v>
       </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>7.5999999999998984</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B85">
         <v>374.08</v>
       </c>
       <c r="C85">
         <v>33.699999999999903</v>
       </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>7.4999999999999041</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B86">
         <v>383.41</v>
       </c>
       <c r="C86">
         <v>33.599999999999902</v>
       </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <f t="shared" si="1"/>
+        <v>7.3999999999999027</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B87">
         <v>387.17</v>
       </c>
       <c r="C87">
         <v>33.499999999999901</v>
       </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <f t="shared" si="1"/>
+        <v>7.2999999999999012</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B88">
         <v>389.08</v>
       </c>
       <c r="C88">
         <v>33.399999999999899</v>
       </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <f t="shared" si="1"/>
+        <v>7.1999999999998998</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B89">
         <v>396.58</v>
       </c>
       <c r="C89">
         <v>33.299999999999898</v>
       </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <f t="shared" si="1"/>
+        <v>7.0999999999998984</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B90">
         <v>400.32</v>
       </c>
       <c r="C90">
         <v>33.199999999999903</v>
       </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <f t="shared" si="1"/>
+        <v>6.9999999999999041</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B91">
         <v>409.66</v>
       </c>
       <c r="C91">
         <v>33.099999999999902</v>
       </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <f t="shared" si="1"/>
+        <v>6.8999999999999027</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B92">
         <v>418.13</v>
       </c>
       <c r="C92">
         <v>32.999999999999901</v>
       </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <f t="shared" si="1"/>
+        <v>6.7999999999999012</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B93">
         <v>421.9</v>
       </c>
       <c r="C93">
         <v>32.899999999999899</v>
       </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <f t="shared" si="1"/>
+        <v>6.6999999999998998</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B94">
         <v>430.36</v>
       </c>
       <c r="C94">
         <v>32.799999999999898</v>
       </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D94">
+        <f t="shared" si="1"/>
+        <v>6.5999999999998984</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B95">
         <v>436.88</v>
       </c>
       <c r="C95">
         <v>32.699999999999903</v>
       </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <f t="shared" si="1"/>
+        <v>6.4999999999999041</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B96">
         <v>447.2</v>
       </c>
       <c r="C96">
         <v>32.599999999999902</v>
       </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D96">
+        <f t="shared" si="1"/>
+        <v>6.3999999999999027</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B97">
         <v>451.81</v>
       </c>
       <c r="C97">
         <v>32.499999999999901</v>
       </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D97">
+        <f t="shared" si="1"/>
+        <v>6.2999999999999012</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B98">
         <v>461.24</v>
       </c>
       <c r="C98">
         <v>32.399999999999899</v>
       </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D98">
+        <f t="shared" si="1"/>
+        <v>6.1999999999998998</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B99">
         <v>470.64</v>
       </c>
       <c r="C99">
         <v>32.299999999999898</v>
       </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <f t="shared" si="1"/>
+        <v>6.0999999999998984</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B100">
         <v>476.28</v>
       </c>
       <c r="C100">
         <v>32.199999999999903</v>
       </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D100">
+        <f t="shared" si="1"/>
+        <v>5.9999999999999041</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B101">
         <v>486.54</v>
       </c>
       <c r="C101">
         <v>32.099999999999902</v>
       </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D101">
+        <f t="shared" si="1"/>
+        <v>5.8999999999999027</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B102">
         <v>490.27</v>
       </c>
       <c r="C102">
         <v>31.999999999999901</v>
       </c>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D102">
+        <f t="shared" si="1"/>
+        <v>5.7999999999999012</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B103">
         <v>502.51</v>
       </c>
       <c r="C103">
         <v>31.899999999999899</v>
       </c>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D103">
+        <f t="shared" si="1"/>
+        <v>5.6999999999998998</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B104">
         <v>508.07</v>
       </c>
       <c r="C104">
         <v>31.799999999999901</v>
       </c>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D104">
+        <f t="shared" si="1"/>
+        <v>5.5999999999999019</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B105">
         <v>519.34</v>
       </c>
       <c r="C105">
         <v>31.6999999999999</v>
       </c>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D105">
+        <f t="shared" si="1"/>
+        <v>5.4999999999999005</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B106">
         <v>529.64</v>
       </c>
       <c r="C106">
         <v>31.599999999999898</v>
       </c>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D106">
+        <f t="shared" si="1"/>
+        <v>5.3999999999998991</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B107">
         <v>536.23</v>
       </c>
       <c r="C107">
         <v>31.499999999999901</v>
       </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D107">
+        <f t="shared" si="1"/>
+        <v>5.2999999999999012</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B108">
         <v>547.52</v>
       </c>
       <c r="C108">
         <v>31.399999999999899</v>
       </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D108">
+        <f t="shared" si="1"/>
+        <v>5.1999999999998998</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B109">
         <v>554.05999999999995</v>
       </c>
       <c r="C109">
         <v>31.299999999999901</v>
       </c>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D109">
+        <f t="shared" si="1"/>
+        <v>5.0999999999999019</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B110">
         <v>565.33000000000004</v>
       </c>
       <c r="C110">
         <v>31.1999999999999</v>
       </c>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D110">
+        <f t="shared" si="1"/>
+        <v>4.9999999999999005</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B111">
         <v>570.9</v>
       </c>
       <c r="C111">
         <v>31.099999999999799</v>
       </c>
-    </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D111">
+        <f t="shared" si="1"/>
+        <v>4.8999999999997996</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B112">
         <v>584.96</v>
       </c>
       <c r="C112">
         <v>30.999999999999801</v>
       </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D112">
+        <f t="shared" si="1"/>
+        <v>4.7999999999998018</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B113">
         <v>598.14</v>
       </c>
       <c r="C113">
         <v>30.8999999999998</v>
       </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D113">
+        <f t="shared" si="1"/>
+        <v>4.6999999999998003</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B114">
         <v>602.75</v>
       </c>
       <c r="C114">
         <v>30.799999999999802</v>
       </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D114">
+        <f t="shared" si="1"/>
+        <v>4.5999999999998025</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B115">
         <v>617.75</v>
       </c>
       <c r="C115">
         <v>30.6999999999998</v>
       </c>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D115">
+        <f t="shared" si="1"/>
+        <v>4.499999999999801</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B116">
         <v>622.5</v>
       </c>
       <c r="C116">
         <v>30.599999999999799</v>
       </c>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D116">
+        <f t="shared" si="1"/>
+        <v>4.3999999999997996</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B117">
         <v>639.30999999999995</v>
       </c>
       <c r="C117">
         <v>30.499999999999801</v>
       </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D117">
+        <f t="shared" si="1"/>
+        <v>4.2999999999998018</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B118">
         <v>643.99</v>
       </c>
       <c r="C118">
         <v>30.3999999999998</v>
       </c>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D118">
+        <f t="shared" si="1"/>
+        <v>4.1999999999998003</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B119">
         <v>657.2</v>
       </c>
       <c r="C119">
         <v>30.299999999999802</v>
       </c>
-    </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D119">
+        <f t="shared" si="1"/>
+        <v>4.0999999999998025</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B120">
         <v>672.21</v>
       </c>
       <c r="C120">
         <v>30.1999999999998</v>
       </c>
-    </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D120">
+        <f t="shared" si="1"/>
+        <v>3.999999999999801</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B121">
         <v>678.75</v>
       </c>
       <c r="C121">
         <v>30.099999999999799</v>
       </c>
-    </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D121">
+        <f t="shared" si="1"/>
+        <v>3.8999999999997996</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B122">
         <v>696.54</v>
       </c>
       <c r="C122">
         <v>29.999999999999801</v>
       </c>
-    </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D122">
+        <f t="shared" si="1"/>
+        <v>3.7999999999998018</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B123">
         <v>704.93</v>
       </c>
       <c r="C123">
         <v>29.8999999999998</v>
       </c>
-    </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D123">
+        <f t="shared" si="1"/>
+        <v>3.6999999999998003</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B124">
         <v>718.17</v>
       </c>
       <c r="C124">
         <v>29.799999999999802</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="1"/>
+        <v>3.5999999999998025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>